<commit_message>
Added support to parse tenant info
</commit_message>
<xml_diff>
--- a/PotentialAnsibleCSVTemplate.xlsx
+++ b/PotentialAnsibleCSVTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joerecchia/Arista/General/CSVtoAVD/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8FB22F46-523D-7541-B42E-832819A93A41}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{204F73D8-AF8A-3B46-B3A4-D02201AB3F3A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2560" yWindow="1040" windowWidth="27640" windowHeight="16940" activeTab="7" xr2:uid="{71463653-0BCE-624A-9151-A855014D3D36}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="188">
   <si>
     <t>Serial Number</t>
   </si>
@@ -229,9 +229,6 @@
     <t>web, app</t>
   </si>
   <si>
-    <t>opzone, web, app, db, vmotion, nfs</t>
-  </si>
-  <si>
     <t>Ethernet1, Ethernet2</t>
   </si>
   <si>
@@ -388,9 +385,6 @@
     <t>Ethernet4, Ethernet4, Ethernet4, Ethernet4</t>
   </si>
   <si>
-    <t>opzone, web, app, db, vmotion, nfs, wan</t>
-  </si>
-  <si>
     <t>DC1-SVC3B</t>
   </si>
   <si>
@@ -475,12 +469,6 @@
     <t>Enabled</t>
   </si>
   <si>
-    <t>TenantA</t>
-  </si>
-  <si>
-    <t>TenantA_OpZone</t>
-  </si>
-  <si>
     <t>10.1.11.1/24</t>
   </si>
   <si>
@@ -496,48 +484,21 @@
     <t>10.1.10.1/24</t>
   </si>
   <si>
-    <t>TenantA_WebZone</t>
-  </si>
-  <si>
     <t>10.1.20.1/24</t>
   </si>
   <si>
-    <t>Tenant_A_Web_Zone_1</t>
-  </si>
-  <si>
     <t>Tenant_A_OP_Zone_2</t>
   </si>
   <si>
-    <t>webzone</t>
-  </si>
-  <si>
-    <t>webzone, erp1</t>
-  </si>
-  <si>
-    <t>Tenant_A_WEBZone_2</t>
-  </si>
-  <si>
     <t>10.1.21.1/24</t>
   </si>
   <si>
-    <t>TenantA_WanZone</t>
-  </si>
-  <si>
     <t>10.1.50.1/24</t>
   </si>
   <si>
     <t>wan</t>
   </si>
   <si>
-    <t>Tenant_A_WANZone_1</t>
-  </si>
-  <si>
-    <t>TenantB</t>
-  </si>
-  <si>
-    <t>TenantB_OpZone</t>
-  </si>
-  <si>
     <t>10.2.10.1/24</t>
   </si>
   <si>
@@ -550,25 +511,97 @@
     <t>Tenant_B_OP_Zone_2</t>
   </si>
   <si>
-    <t>TenantB_WANZone</t>
-  </si>
-  <si>
     <t>10.2.50.1/24</t>
   </si>
   <si>
     <t>Tenant_B_WAN_Zone_1</t>
   </si>
   <si>
-    <t>TenantC</t>
-  </si>
-  <si>
-    <t>TenantC_OpZone</t>
-  </si>
-  <si>
     <t>10.3.10.1/24</t>
   </si>
   <si>
     <t>Tenant_C_OP_Zone_1</t>
+  </si>
+  <si>
+    <t>web</t>
+  </si>
+  <si>
+    <t>web, erp1</t>
+  </si>
+  <si>
+    <t>app</t>
+  </si>
+  <si>
+    <t>app, erp1</t>
+  </si>
+  <si>
+    <t>10.1.30.1/24</t>
+  </si>
+  <si>
+    <t>10.1.31.1/24</t>
+  </si>
+  <si>
+    <t>Tenant_A_APP_Zone_2</t>
+  </si>
+  <si>
+    <t>Tenant_A_WEB_Zone_2</t>
+  </si>
+  <si>
+    <t>Tenant_B_WAN_Zone</t>
+  </si>
+  <si>
+    <t>Tenant_A_DB_Zone</t>
+  </si>
+  <si>
+    <t>10.1.40.1/24</t>
+  </si>
+  <si>
+    <t>Tenant_A_DB_Zone_1</t>
+  </si>
+  <si>
+    <t>Tenant_A_APP_Zone_1</t>
+  </si>
+  <si>
+    <t>db</t>
+  </si>
+  <si>
+    <t>10.1.41.1/24</t>
+  </si>
+  <si>
+    <t>Tenant_A_DB_Zone_2</t>
+  </si>
+  <si>
+    <t>opzone, web, app, db</t>
+  </si>
+  <si>
+    <t>Tenant_B</t>
+  </si>
+  <si>
+    <t>Tenant_C</t>
+  </si>
+  <si>
+    <t>Tenant_A_OP_Zone</t>
+  </si>
+  <si>
+    <t>Tenant_A_WEB_Zone</t>
+  </si>
+  <si>
+    <t>Tenant_A_APP_Zone</t>
+  </si>
+  <si>
+    <t>Tenant_A_WAN_Zone</t>
+  </si>
+  <si>
+    <t>Tenant_B_OP_Zone</t>
+  </si>
+  <si>
+    <t>Tenant_C_OP_Zone</t>
+  </si>
+  <si>
+    <t>Tenant_A_WEB_Zone_1</t>
+  </si>
+  <si>
+    <t>Tenant_A_WAN_Zone_1</t>
   </si>
 </sst>
 </file>
@@ -1035,58 +1068,58 @@
         <v>10</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>85</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="C6" s="15" t="s">
         <v>86</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="C6" s="15" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -1160,7 +1193,7 @@
         <v>29</v>
       </c>
       <c r="C15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -1168,7 +1201,7 @@
         <v>30</v>
       </c>
       <c r="C16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -1176,7 +1209,7 @@
         <v>31</v>
       </c>
       <c r="C17" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -1213,37 +1246,37 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B22" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B23" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C24" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
+        <v>87</v>
+      </c>
+      <c r="C25" t="s">
         <v>88</v>
-      </c>
-      <c r="C25" t="s">
-        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -1300,7 +1333,7 @@
         <v>43</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -1312,7 +1345,7 @@
         <v>44</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -1381,10 +1414,10 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -1392,7 +1425,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -1405,10 +1438,10 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -1420,9 +1453,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{729B4815-0CB8-AC46-AFED-71170ED8249A}">
   <dimension ref="A1:AA8"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+    <sheetView topLeftCell="K1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:XFD1"/>
+      <selection pane="bottomLeft" activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1465,16 +1498,16 @@
         <v>4</v>
       </c>
       <c r="H1" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="I1" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="J1" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="J1" s="13" t="s">
+      <c r="K1" s="13" t="s">
         <v>69</v>
-      </c>
-      <c r="K1" s="13" t="s">
-        <v>70</v>
       </c>
       <c r="L1" s="13" t="s">
         <v>20</v>
@@ -1521,7 +1554,7 @@
       <c r="I2" s="10"/>
       <c r="J2" s="6"/>
       <c r="K2" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="L2" s="11" t="s">
         <v>60</v>
@@ -1557,13 +1590,13 @@
       <c r="I3" s="10"/>
       <c r="J3" s="6"/>
       <c r="K3" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="L3" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="M3" s="11" t="s">
-        <v>63</v>
+      <c r="M3" s="6" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.2">
@@ -1593,13 +1626,13 @@
       <c r="I4" s="10"/>
       <c r="J4" s="6"/>
       <c r="K4" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="L4" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="M4" s="11" t="s">
-        <v>63</v>
+      <c r="M4" s="6" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.2">
@@ -1608,20 +1641,20 @@
         <v>4</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C5" s="10"/>
       <c r="D5" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="E5" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="E5" s="14" t="s">
+      <c r="F5" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="F5" s="11" t="s">
+      <c r="G5" s="16" t="s">
         <v>113</v>
-      </c>
-      <c r="G5" s="16" t="s">
-        <v>114</v>
       </c>
       <c r="H5" s="10">
         <v>65103</v>
@@ -1629,13 +1662,13 @@
       <c r="I5" s="10"/>
       <c r="J5" s="6"/>
       <c r="K5" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="L5" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="M5" s="11" t="s">
-        <v>116</v>
+      <c r="M5" s="6" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.2">
@@ -1644,20 +1677,20 @@
         <v>5</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C6" s="10"/>
       <c r="D6" s="14" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F6" s="11" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H6" s="10">
         <v>65103</v>
@@ -1665,13 +1698,13 @@
       <c r="I6" s="10"/>
       <c r="J6" s="6"/>
       <c r="K6" s="6" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="L6" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="M6" s="11" t="s">
-        <v>116</v>
+      <c r="M6" s="6" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.2">
@@ -1738,28 +1771,28 @@
         <v>19</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B5" s="7"/>
     </row>
@@ -1771,15 +1804,15 @@
     </row>
     <row r="7" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B8" s="10" t="s">
         <v>24</v>
@@ -1787,7 +1820,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B9" s="10">
         <v>16384</v>
@@ -1798,7 +1831,7 @@
         <v>7</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -1811,7 +1844,7 @@
     </row>
     <row r="12" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B12" s="10" t="b">
         <v>0</v>
@@ -1826,9 +1859,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41311A7A-7CCF-024D-AE59-C5F21012B3DE}">
   <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+    <sheetView topLeftCell="I1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:XFD1"/>
+      <selection pane="bottomLeft" activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1873,10 +1906,10 @@
         <v>22</v>
       </c>
       <c r="I1" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="J1" s="7" t="s">
         <v>76</v>
-      </c>
-      <c r="J1" s="7" t="s">
-        <v>77</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>20</v>
@@ -1890,31 +1923,31 @@
         <v>8</v>
       </c>
       <c r="B2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="F2" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="H2" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="I2" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="J2" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="K2" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="I2" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="J2" s="6" t="s">
+      <c r="L2" s="6" t="s">
         <v>125</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
@@ -1923,28 +1956,28 @@
         <v>9</v>
       </c>
       <c r="B3" t="s">
+        <v>126</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="E3" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="F3" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="G3" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="H3" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="G3" s="6" t="s">
-        <v>132</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>133</v>
-      </c>
       <c r="I3" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
@@ -1953,28 +1986,28 @@
         <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E4" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="J4" s="6" t="s">
         <v>134</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>132</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="J4" s="6" t="s">
-        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -2010,18 +2043,18 @@
         <v>19</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="17" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B3" s="17"/>
     </row>
     <row r="4" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="17" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B4" s="17"/>
     </row>
@@ -2033,7 +2066,7 @@
     </row>
     <row r="6" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B6" s="10" t="s">
         <v>24</v>
@@ -2041,7 +2074,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B7" s="10">
         <v>16384</v>
@@ -2054,11 +2087,11 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B85D48BE-CB72-BC43-A02D-945523B5A1A7}">
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="125" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
+      <selection pane="bottomLeft" activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2077,45 +2110,45 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B1" t="s">
         <v>138</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D1" t="s">
+        <v>139</v>
+      </c>
+      <c r="E1" t="s">
         <v>140</v>
       </c>
-      <c r="C1" t="s">
-        <v>139</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
+        <v>146</v>
+      </c>
+      <c r="G1" t="s">
         <v>141</v>
       </c>
-      <c r="E1" t="s">
-        <v>142</v>
-      </c>
-      <c r="F1" t="s">
-        <v>150</v>
-      </c>
-      <c r="G1" t="s">
-        <v>143</v>
-      </c>
       <c r="H1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I1" t="s">
         <v>21</v>
       </c>
       <c r="J1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>145</v>
+        <v>124</v>
       </c>
       <c r="B2">
         <v>10000</v>
       </c>
       <c r="C2" t="s">
-        <v>146</v>
+        <v>180</v>
       </c>
       <c r="D2">
         <v>10</v>
@@ -2124,13 +2157,13 @@
         <v>110</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="I2" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="J2" t="b">
         <v>1</v>
@@ -2138,13 +2171,13 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>145</v>
+        <v>124</v>
       </c>
       <c r="B3">
         <v>10000</v>
       </c>
       <c r="C3" t="s">
-        <v>146</v>
+        <v>180</v>
       </c>
       <c r="D3">
         <v>10</v>
@@ -2156,13 +2189,13 @@
         <v>50111</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="I3" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="J3" t="b">
         <v>1</v>
@@ -2170,13 +2203,13 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>145</v>
+        <v>124</v>
       </c>
       <c r="B4">
         <v>10000</v>
       </c>
       <c r="C4" t="s">
-        <v>152</v>
+        <v>181</v>
       </c>
       <c r="D4">
         <v>11</v>
@@ -2186,13 +2219,13 @@
       </c>
       <c r="F4" s="19"/>
       <c r="G4" s="6" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>154</v>
+        <v>186</v>
       </c>
       <c r="I4" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="J4" t="b">
         <v>1</v>
@@ -2200,13 +2233,13 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>145</v>
+        <v>124</v>
       </c>
       <c r="B5">
         <v>10000</v>
       </c>
       <c r="C5" t="s">
-        <v>152</v>
+        <v>181</v>
       </c>
       <c r="D5">
         <v>11</v>
@@ -2216,13 +2249,13 @@
       </c>
       <c r="F5" s="19"/>
       <c r="G5" s="6" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>158</v>
+        <v>168</v>
       </c>
       <c r="I5" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
       <c r="J5" t="b">
         <v>1</v>
@@ -2230,29 +2263,29 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>145</v>
+        <v>124</v>
       </c>
       <c r="B6">
         <v>10000</v>
       </c>
       <c r="C6" t="s">
-        <v>160</v>
+        <v>182</v>
       </c>
       <c r="D6">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E6">
-        <v>150</v>
+        <v>130</v>
       </c>
       <c r="F6" s="19"/>
       <c r="G6" s="6" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>163</v>
-      </c>
-      <c r="I6" t="s">
-        <v>162</v>
+        <v>173</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>164</v>
       </c>
       <c r="J6" t="b">
         <v>1</v>
@@ -2260,28 +2293,29 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>164</v>
+        <v>124</v>
       </c>
       <c r="B7">
-        <v>20000</v>
+        <v>10000</v>
       </c>
       <c r="C7" t="s">
-        <v>165</v>
+        <v>182</v>
       </c>
       <c r="D7">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="E7">
-        <v>210</v>
-      </c>
+        <v>131</v>
+      </c>
+      <c r="F7" s="19"/>
       <c r="G7" s="6" t="s">
         <v>166</v>
       </c>
       <c r="H7" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="I7" t="s">
-        <v>149</v>
+      <c r="I7" s="6" t="s">
+        <v>163</v>
       </c>
       <c r="J7" t="b">
         <v>1</v>
@@ -2289,28 +2323,29 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>164</v>
+        <v>124</v>
       </c>
       <c r="B8">
-        <v>20000</v>
+        <v>10000</v>
       </c>
       <c r="C8" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="D8">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="E8">
-        <v>211</v>
-      </c>
+        <v>140</v>
+      </c>
+      <c r="F8" s="19"/>
       <c r="G8" s="6" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="I8" t="s">
-        <v>149</v>
+        <v>172</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>174</v>
       </c>
       <c r="J8" t="b">
         <v>1</v>
@@ -2318,28 +2353,29 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>164</v>
+        <v>124</v>
       </c>
       <c r="B9">
-        <v>20000</v>
+        <v>10000</v>
       </c>
       <c r="C9" t="s">
         <v>170</v>
       </c>
       <c r="D9">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="E9">
-        <v>250</v>
-      </c>
+        <v>141</v>
+      </c>
+      <c r="F9" s="19"/>
       <c r="G9" s="6" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>172</v>
-      </c>
-      <c r="I9" t="s">
-        <v>162</v>
+        <v>176</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>174</v>
       </c>
       <c r="J9" t="b">
         <v>1</v>
@@ -2347,30 +2383,147 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>173</v>
+        <v>124</v>
       </c>
       <c r="B10">
+        <v>10000</v>
+      </c>
+      <c r="C10" t="s">
+        <v>183</v>
+      </c>
+      <c r="D10">
+        <v>14</v>
+      </c>
+      <c r="E10">
+        <v>150</v>
+      </c>
+      <c r="F10" s="19"/>
+      <c r="G10" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="I10" t="s">
+        <v>152</v>
+      </c>
+      <c r="J10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>178</v>
+      </c>
+      <c r="B11">
+        <v>20000</v>
+      </c>
+      <c r="C11" t="s">
+        <v>184</v>
+      </c>
+      <c r="D11">
+        <v>20</v>
+      </c>
+      <c r="E11">
+        <v>210</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="I11" t="s">
+        <v>145</v>
+      </c>
+      <c r="J11" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>178</v>
+      </c>
+      <c r="B12">
+        <v>20000</v>
+      </c>
+      <c r="C12" t="s">
+        <v>184</v>
+      </c>
+      <c r="D12">
+        <v>20</v>
+      </c>
+      <c r="E12">
+        <v>211</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="I12" t="s">
+        <v>145</v>
+      </c>
+      <c r="J12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>178</v>
+      </c>
+      <c r="B13">
+        <v>20000</v>
+      </c>
+      <c r="C13" t="s">
+        <v>169</v>
+      </c>
+      <c r="D13">
+        <v>21</v>
+      </c>
+      <c r="E13">
+        <v>250</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="I13" t="s">
+        <v>152</v>
+      </c>
+      <c r="J13" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>179</v>
+      </c>
+      <c r="B14">
         <v>30000</v>
       </c>
-      <c r="C10" t="s">
-        <v>174</v>
-      </c>
-      <c r="D10">
+      <c r="C14" t="s">
+        <v>185</v>
+      </c>
+      <c r="D14">
         <v>30</v>
       </c>
-      <c r="E10">
+      <c r="E14">
         <v>310</v>
       </c>
-      <c r="G10" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="H10" s="6" t="s">
-        <v>176</v>
-      </c>
-      <c r="I10" t="s">
-        <v>149</v>
-      </c>
-      <c r="J10" t="b">
+      <c r="G14" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="I14" t="s">
+        <v>145</v>
+      </c>
+      <c r="J14" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added support to parse server/port-profile info
</commit_message>
<xml_diff>
--- a/PotentialAnsibleCSVTemplate.xlsx
+++ b/PotentialAnsibleCSVTemplate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joerecchia/Arista/General/CSVtoAVD/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{204F73D8-AF8A-3B46-B3A4-D02201AB3F3A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBFE7F24-5DED-AA48-BBE5-8670BB2B6DD9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2560" yWindow="1040" windowWidth="27640" windowHeight="16940" activeTab="7" xr2:uid="{71463653-0BCE-624A-9151-A855014D3D36}"/>
+    <workbookView xWindow="2560" yWindow="1040" windowWidth="27640" windowHeight="16940" firstSheet="1" activeTab="8" xr2:uid="{71463653-0BCE-624A-9151-A855014D3D36}"/>
   </bookViews>
   <sheets>
     <sheet name="General Configuration Details" sheetId="5" r:id="rId1"/>
@@ -21,6 +21,8 @@
     <sheet name="L2 Leaf Info" sheetId="8" r:id="rId6"/>
     <sheet name="L2 Leaf Configuration Details" sheetId="7" r:id="rId7"/>
     <sheet name="Tenants" sheetId="6" r:id="rId8"/>
+    <sheet name="Port Profiles" sheetId="9" r:id="rId9"/>
+    <sheet name="Servers" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029" calcOnSave="0"/>
   <extLst>
@@ -38,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="225">
   <si>
     <t>Serial Number</t>
   </si>
@@ -602,6 +604,117 @@
   </si>
   <si>
     <t>Tenant_A_WAN_Zone_1</t>
+  </si>
+  <si>
+    <t>Port Profile</t>
+  </si>
+  <si>
+    <t>Mode</t>
+  </si>
+  <si>
+    <t>Vlans</t>
+  </si>
+  <si>
+    <t>Server</t>
+  </si>
+  <si>
+    <t>Rack</t>
+  </si>
+  <si>
+    <t>Adapter</t>
+  </si>
+  <si>
+    <t>Server Ports</t>
+  </si>
+  <si>
+    <t>Switch Ports</t>
+  </si>
+  <si>
+    <t>Switches</t>
+  </si>
+  <si>
+    <t>Port-Channel</t>
+  </si>
+  <si>
+    <t>Port-Channel Mode</t>
+  </si>
+  <si>
+    <t>TENANT_A_B</t>
+  </si>
+  <si>
+    <t>TENANT_A</t>
+  </si>
+  <si>
+    <t>TENANT_B</t>
+  </si>
+  <si>
+    <t>110-111,210-211</t>
+  </si>
+  <si>
+    <t>210-211</t>
+  </si>
+  <si>
+    <t>server01</t>
+  </si>
+  <si>
+    <t>RackB</t>
+  </si>
+  <si>
+    <t>Eth1</t>
+  </si>
+  <si>
+    <t>Ethernet5</t>
+  </si>
+  <si>
+    <t>Eth4, Eth5</t>
+  </si>
+  <si>
+    <t>Ethernet7, Ethernet8</t>
+  </si>
+  <si>
+    <t>DC1-LEAF1A, DC1-LEAF1A</t>
+  </si>
+  <si>
+    <t>PortChannel1</t>
+  </si>
+  <si>
+    <t>active</t>
+  </si>
+  <si>
+    <t>Eth2, Eth3</t>
+  </si>
+  <si>
+    <t>Ethernet10, Ethernet10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DC1-LEAF2A, DC1-LEAF2B </t>
+  </si>
+  <si>
+    <t>server02</t>
+  </si>
+  <si>
+    <t>Ethernet6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eth2, Eth3 </t>
+  </si>
+  <si>
+    <t>Ethernet11, Ethernet11</t>
+  </si>
+  <si>
+    <t>server03</t>
+  </si>
+  <si>
+    <t>RackC</t>
+  </si>
+  <si>
+    <t>Eth1, Eth2</t>
+  </si>
+  <si>
+    <t>server04</t>
+  </si>
+  <si>
+    <t>trunk</t>
   </si>
 </sst>
 </file>
@@ -1284,6 +1397,252 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08ACCC69-7B6B-8B45-B58C-2055E380561D}">
+  <dimension ref="A1:I8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I1" sqref="I1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B1" t="s">
+        <v>192</v>
+      </c>
+      <c r="C1" t="s">
+        <v>193</v>
+      </c>
+      <c r="D1" t="s">
+        <v>194</v>
+      </c>
+      <c r="E1" t="s">
+        <v>195</v>
+      </c>
+      <c r="F1" t="s">
+        <v>196</v>
+      </c>
+      <c r="G1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H1" t="s">
+        <v>197</v>
+      </c>
+      <c r="I1" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>212</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBBCDCF0-A743-DF46-BE03-0406672D0FEF}">
   <dimension ref="A1:I5"/>
@@ -1453,7 +1812,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{729B4815-0CB8-AC46-AFED-71170ED8249A}">
   <dimension ref="A1:AA8"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="M6" sqref="M6"/>
     </sheetView>
@@ -2089,7 +2448,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B85D48BE-CB72-BC43-A02D-945523B5A1A7}">
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="125" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="125" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="H11" sqref="H11"/>
     </sheetView>
@@ -2530,4 +2889,67 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{397623ED-C334-C646-B5F8-79A547B3D517}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>188</v>
+      </c>
+      <c r="B1" t="s">
+        <v>189</v>
+      </c>
+      <c r="C1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>199</v>
+      </c>
+      <c r="B2" t="s">
+        <v>224</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="B3" t="s">
+        <v>224</v>
+      </c>
+      <c r="C3" s="6">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="B4" t="s">
+        <v>224</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>203</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>